<commit_message>
Exercise done with original challenge.xlsx file
Exercise done with original challenge.xlsx file
</commit_message>
<xml_diff>
--- a/resources/challange.xlsx
+++ b/resources/challange.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\Automation_Challange_Robot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86EBD32-1423-44AA-A193-B9B71F271AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C75E74-8415-4065-AD7D-586442D76808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>Gwendolin</t>
   </si>
@@ -218,13 +219,154 @@
   </si>
   <si>
     <t>kupleyband9@opera.com</t>
+  </si>
+  <si>
+    <t>Role in Company</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>98 North Road</t>
+  </si>
+  <si>
+    <t>jsmith@itsolutions.co.uk</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Dorsey</t>
+  </si>
+  <si>
+    <t>11 Crown Street</t>
+  </si>
+  <si>
+    <t>jdorsey@mc.com</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Kipling</t>
+  </si>
+  <si>
+    <t>Waterfront</t>
+  </si>
+  <si>
+    <t>22 Guild Street</t>
+  </si>
+  <si>
+    <t>kipling@waterfront.com</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Robertson</t>
+  </si>
+  <si>
+    <t>17 Farburn Terrace</t>
+  </si>
+  <si>
+    <t>mrobertson@mc.com</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>Derrick</t>
+  </si>
+  <si>
+    <t>Timepath Inc.</t>
+  </si>
+  <si>
+    <t>99 Shire Oak Road</t>
+  </si>
+  <si>
+    <t>dderrick@timepath.co.uk</t>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t>Marlowe</t>
+  </si>
+  <si>
+    <t>27 Cheshire Street</t>
+  </si>
+  <si>
+    <t>jmarlowe@aperture.us</t>
+  </si>
+  <si>
+    <t>Stan</t>
+  </si>
+  <si>
+    <t>Hamm</t>
+  </si>
+  <si>
+    <t>Sugarwell</t>
+  </si>
+  <si>
+    <t>Advisor</t>
+  </si>
+  <si>
+    <t>10 Dam Road</t>
+  </si>
+  <si>
+    <t>shamm@sugarwell.org</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>13 White Rabbit Street</t>
+  </si>
+  <si>
+    <t>mnorton@aperture.us</t>
+  </si>
+  <si>
+    <t>Stacy</t>
+  </si>
+  <si>
+    <t>Shelby</t>
+  </si>
+  <si>
+    <t>HR Manager</t>
+  </si>
+  <si>
+    <t>19 Pineapple Boulevard</t>
+  </si>
+  <si>
+    <t>sshelby@techdev.com</t>
+  </si>
+  <si>
+    <t>Lara</t>
+  </si>
+  <si>
+    <t>Palmer</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>87 Orange Street</t>
+  </si>
+  <si>
+    <t>lpalmer@timepath.co.uk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,8 +509,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,8 +700,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -664,8 +822,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -709,16 +904,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -757,6 +964,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{90419E83-FEEA-4C83-89DD-C68543E1D627}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1076,7 +1284,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G11" sqref="G2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1298,285 @@
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="8">
+        <v>40716543298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="8">
+        <v>40791345621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="8">
+        <v>40735416854</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="8">
+        <v>40733652145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="8">
+        <v>40799885412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="8">
+        <v>40733154268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="8">
+        <v>40712462257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="8">
+        <v>40731254562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="8">
+        <v>40741785214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="8">
+        <v>40731653845</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63A0F8A-4C3C-4326-AA8E-1A1DBBBBB0B9}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1345,12 +1831,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{F890FAC8-98A2-4D65-90DA-F357980EF513}"/>
-    <hyperlink ref="F9" r:id="rId2" xr:uid="{4171ACAD-8D63-4D95-9489-4FCE8FCFC355}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{D0C9FC65-BE99-4CA8-8E3E-7B7BB08C385A}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{0DB354C9-E7DC-4FC1-8235-760A06E3F022}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{0DB354C9-E7DC-4FC1-8235-760A06E3F022}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{D0C9FC65-BE99-4CA8-8E3E-7B7BB08C385A}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{4171ACAD-8D63-4D95-9489-4FCE8FCFC355}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{F890FAC8-98A2-4D65-90DA-F357980EF513}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>